<commit_message>
Adição de novas tabelas de banco
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\powerjob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4BE491-13D6-46A5-8B49-09EE0F026ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1BE5B3-6D12-4CF2-9AA5-0403DBA0A2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{1C37741A-9682-4B72-BC63-DDF2148DC411}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{1C37741A-9682-4B72-BC63-DDF2148DC411}"/>
   </bookViews>
   <sheets>
     <sheet name="Cotacoes" sheetId="1" r:id="rId1"/>
     <sheet name="Portal" sheetId="4" r:id="rId2"/>
     <sheet name="API" sheetId="5" r:id="rId3"/>
+    <sheet name="Banco de Dados" sheetId="6" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="rng_completedPercent">[1]License!$D$1125</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="45">
   <si>
     <t>Status</t>
   </si>
@@ -142,9 +143,6 @@
     <t>Criação da tela de login</t>
   </si>
   <si>
-    <t>Aguardando</t>
-  </si>
-  <si>
     <t>Criação da consulta dos dados para autenticação do usuário</t>
   </si>
   <si>
@@ -160,14 +158,35 @@
     <t>Criação da tabela status das cotações</t>
   </si>
   <si>
-    <t>Fin</t>
+    <t>Fase 2</t>
+  </si>
+  <si>
+    <t>Criação da tela de cards</t>
+  </si>
+  <si>
+    <t>Aguardando</t>
+  </si>
+  <si>
+    <t>Criação da consulta de cotações para a empresa</t>
+  </si>
+  <si>
+    <t>Criação do processo de relacionamento de eventos com a empresa</t>
+  </si>
+  <si>
+    <t>Criação da tabela de relacionamento de eventos com a empresa</t>
+  </si>
+  <si>
+    <t>Criação da tabela para registro de autenticação por portal de cotação</t>
+  </si>
+  <si>
+    <t>Criação da tabela para registro de portais disponíveis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,8 +232,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +260,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -303,11 +336,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,11 +437,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -559,10 +690,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -748,6 +879,819 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Tarefas por prioridade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Banco de Dados'!$J$5:$J$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>P0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>P1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>P2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Banco de Dados'!$K$5:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B937-4D9D-B465-F21CA28B4541}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2069350255"/>
+        <c:axId val="2069350735"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2069350255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069350735"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2069350735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069350255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-55EC-4CB8-82CC-4BC116E4DD4F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-55EC-4CB8-82CC-4BC116E4DD4F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Banco de Dados'!$T$6:$T$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Finalizadas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total Geral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Banco de Dados'!$U$6:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-55EC-4CB8-82CC-4BC116E4DD4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1548-4550-A2E4-60C6CAEC195B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1548-4550-A2E4-60C6CAEC195B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Banco de Dados'!$T$10:$T$11</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Finalizadas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Prioridade 0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Banco de Dados'!$U$10:$U$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1548-4550-A2E4-60C6CAEC195B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -900,10 +1844,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1151,7 +2095,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1372,7 +2316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -1713,7 +2657,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -1967,7 +2911,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2185,7 +3129,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2526,7 +3470,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -2777,7 +3721,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -2877,6 +3821,126 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3739,6 +4803,1543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
@@ -8198,6 +10799,125 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{821D537F-7C79-4EC9-8517-2FEEE229FE29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC672E07-2FB3-4AAF-BF48-B9E7AC4B484C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92574186-DD2B-4108-8366-64BEF11847F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -8524,7 +11244,7 @@
   <dimension ref="B1:U39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8611,13 +11331,13 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="14">
         <v>0</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>20</v>
@@ -8634,23 +11354,23 @@
       </c>
       <c r="K5" s="9">
         <f>COUNTIF(C:C,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5" s="9">
         <f>COUNTIFS($E:$E,"Finalizada",$C:$C,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T5" t="s">
         <v>17</v>
       </c>
       <c r="U5">
         <f>K9</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" s="14">
         <v>0</v>
@@ -8667,13 +11387,13 @@
       <c r="G6" s="15">
         <v>100</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="16"/>
       <c r="J6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="9">
         <f>COUNTIF(C:C,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="9">
         <f>COUNTIFS($E:$E,"Finalizada",$C:$C,1)</f>
@@ -8684,15 +11404,15 @@
       </c>
       <c r="U6">
         <f>L9</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>19</v>
@@ -8723,29 +11443,21 @@
       </c>
       <c r="U7">
         <f>U5-U6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="14">
-        <v>0</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="15">
-        <v>100</v>
-      </c>
-      <c r="H8" s="16"/>
+      <c r="B8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23">
+        <v>0</v>
+      </c>
+      <c r="H8" s="22"/>
       <c r="J8" s="9" t="s">
         <v>16</v>
       </c>
@@ -8759,54 +11471,54 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="B9" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="26">
         <v>1</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="15" t="s">
+      <c r="D9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="15">
-        <v>100</v>
-      </c>
-      <c r="H9" s="14"/>
+      <c r="G9" s="27">
+        <v>0</v>
+      </c>
+      <c r="H9" s="26"/>
       <c r="J9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="11">
         <f>SUM(K5:K8)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L9" s="11">
         <f>SUM(L5:L8)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T9" t="s">
         <v>9</v>
       </c>
       <c r="U9">
         <f>K5</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34">
+        <v>0</v>
+      </c>
+      <c r="H10" s="33"/>
       <c r="J10" s="12"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -8815,19 +11527,19 @@
       </c>
       <c r="U10">
         <f>L5</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34">
+        <v>0</v>
+      </c>
+      <c r="H11" s="33"/>
       <c r="T11" t="s">
         <v>9</v>
       </c>
@@ -8837,15 +11549,15 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30">
+        <v>0</v>
+      </c>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
@@ -9152,16 +11864,16 @@
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="B1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Em andamento">
+  <conditionalFormatting sqref="E12:E1048576 E1:E9">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",E1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -9173,7 +11885,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -9185,7 +11897,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9199,7 +11911,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G39">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -9280,8 +11992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF942F75-EA4F-4CDF-B916-D61FB5178533}">
   <dimension ref="B1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9391,7 +12103,7 @@
       </c>
       <c r="K5" s="9">
         <f>COUNTIF(C:C,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" s="9">
         <f>COUNTIFS($E:$E,"Finalizada",$C:$C,0)</f>
@@ -9402,7 +12114,7 @@
       </c>
       <c r="U5">
         <f>K9</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
@@ -9416,13 +12128,13 @@
         <v>23</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H6" s="14"/>
       <c r="J6" s="9" t="s">
@@ -9434,19 +12146,19 @@
       </c>
       <c r="L6" s="9">
         <f>COUNTIFS($E:$E,"Finalizada",$C:$C,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T6" t="s">
         <v>12</v>
       </c>
       <c r="U6">
         <f>L9</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="14">
         <v>0</v>
@@ -9485,7 +12197,7 @@
     </row>
     <row r="8" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="14">
         <v>0</v>
@@ -9517,7 +12229,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="14">
         <v>0</v>
@@ -9540,23 +12252,23 @@
       </c>
       <c r="K9" s="11">
         <f>SUM(K5:K8)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L9" s="11">
         <f>SUM(L5:L8)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T9" t="s">
         <v>9</v>
       </c>
       <c r="U9">
         <f>K5</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="14">
         <v>0</v>
@@ -9586,29 +12298,41 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14"/>
+      <c r="B11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
+      <c r="H11" s="22"/>
       <c r="T11" t="s">
         <v>9</v>
       </c>
       <c r="U11">
         <f>U9-U10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="B12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G12" s="15">
         <v>0</v>
       </c>
@@ -9920,10 +12644,10 @@
     <mergeCell ref="K10:L10"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",E1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10048,7 +12772,7 @@
   <dimension ref="B1:U39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10135,7 +12859,7 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="14">
         <v>0</v>
@@ -10144,7 +12868,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>21</v>
@@ -10158,30 +12882,32 @@
       </c>
       <c r="K5" s="9">
         <f>COUNTIF(C:C,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" s="9">
         <f>COUNTIFS($E:$E,"Finalizada",$C:$C,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" t="s">
         <v>17</v>
       </c>
       <c r="U5">
         <f>K9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14"/>
+      <c r="B6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23">
+        <v>0</v>
+      </c>
+      <c r="H6" s="22"/>
       <c r="J6" s="9" t="s">
         <v>14</v>
       </c>
@@ -10198,15 +12924,25 @@
       </c>
       <c r="U6">
         <f>L9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G7" s="15">
         <v>0</v>
       </c>
@@ -10267,18 +13003,18 @@
       </c>
       <c r="K9" s="11">
         <f>SUM(K5:K8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="11">
         <f>SUM(L5:L8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" t="s">
         <v>9</v>
       </c>
       <c r="U9">
         <f>K5</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
@@ -10299,7 +13035,7 @@
       </c>
       <c r="U10">
         <f>L5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
@@ -10637,10 +13373,10 @@
     <mergeCell ref="K10:L10"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",E1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10758,4 +13494,763 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12350CF4-F513-49CF-93E7-214C7539DEBA}">
+  <dimension ref="B1:U39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="1.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="5.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="J1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+    </row>
+    <row r="2" spans="2:21" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="15">
+        <v>100</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="J5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="9">
+        <f>COUNTIF(C:C,0)</f>
+        <v>5</v>
+      </c>
+      <c r="L5" s="9">
+        <f>COUNTIFS($E:$E,"Finalizada",$C:$C,0)</f>
+        <v>5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U5">
+        <f>K9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="15">
+        <v>100</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="J6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="9">
+        <f>COUNTIF(C:C,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <f>COUNTIFS($E:$E,"Finalizada",$C:$C,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6">
+        <f>L9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9">
+        <f>COUNTIF(C:C,2)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <f>COUNTIFS($E:$E,"Finalizada",$C:$C,2)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7">
+        <f>U5-U6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="15">
+        <v>100</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="J8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="9">
+        <f>COUNTIF(C:C,3)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <f>COUNTIFS($E:$E,"Finalizada",$C:$C,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="27">
+        <v>100</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="J9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="11">
+        <f>SUM(K5:K8)</f>
+        <v>5</v>
+      </c>
+      <c r="L9" s="11">
+        <f>SUM(L5:L8)</f>
+        <v>5</v>
+      </c>
+      <c r="T9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9">
+        <f>K5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="27">
+        <v>100</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="T10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10">
+        <f>L5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="T11" t="s">
+        <v>9</v>
+      </c>
+      <c r="U11">
+        <f>U9-U10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27">
+        <v>0</v>
+      </c>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27">
+        <v>0</v>
+      </c>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27">
+        <v>0</v>
+      </c>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15">
+        <v>0</v>
+      </c>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15">
+        <v>0</v>
+      </c>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15">
+        <v>0</v>
+      </c>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15">
+        <v>0</v>
+      </c>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15">
+        <v>0</v>
+      </c>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15">
+        <v>0</v>
+      </c>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15">
+        <v>0</v>
+      </c>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15">
+        <v>0</v>
+      </c>
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15">
+        <v>0</v>
+      </c>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15">
+        <v>0</v>
+      </c>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15">
+        <v>0</v>
+      </c>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="13"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15">
+        <v>0</v>
+      </c>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15">
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15">
+        <v>0</v>
+      </c>
+      <c r="H39" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="K10:L10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",E1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="dataBar" priority="52">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color theme="8" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2DDDAE6C-A87A-4E3C-941E-0CAC6E6C6F20}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="dataBar" priority="53">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8E820104-645B-492D-9F9E-8459EECFFCCC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="dataBar" priority="54">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{26574793-A703-4E56-8888-EDEF6CDCFDCB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G39">
+    <cfRule type="dataBar" priority="64">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color theme="8" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3FFA1975-9CB9-4530-9CD7-94A3B9FFA346}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2DDDAE6C-A87A-4E3C-941E-0CAC6E6C6F20}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{8E820104-645B-492D-9F9E-8459EECFFCCC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{26574793-A703-4E56-8888-EDEF6CDCFDCB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3FFA1975-9CB9-4530-9CD7-94A3B9FFA346}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G5:G39</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>